<commit_message>
update chapter 4 again
</commit_message>
<xml_diff>
--- a/contoh/data.xlsx
+++ b/contoh/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -554,7 +554,7 @@
   </sheetPr>
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -1045,7 +1045,7 @@
   <dimension ref="B2:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1133,8 +1133,8 @@
   </sheetPr>
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>